<commit_message>
clarify a few points
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -50,15 +50,19 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Ken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
+    <numFmt formatCode="DD/MM/YY" numFmtId="166"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -125,9 +129,10 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -145,10 +150,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I3" activeCellId="0" pane="topLeft" sqref="I3"/>
+      <selection activeCell="G4" activeCellId="0" pane="topLeft" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -220,12 +225,29 @@
         <f aca="false">D3/C3</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">C3*C3</f>
-        <v>49</v>
-      </c>
       <c r="I3" s="0" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
+        <v>42037</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">D5/C5</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>